<commit_message>
Update new set of slides
</commit_message>
<xml_diff>
--- a/Participants2016.xlsx
+++ b/Participants2016.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="100" windowWidth="24920" windowHeight="12340"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="24915" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>First name</t>
   </si>
@@ -149,13 +149,22 @@
   </si>
   <si>
     <t>j2.montanus@student.vu.nl</t>
+  </si>
+  <si>
+    <t>Aldida</t>
+  </si>
+  <si>
+    <t>Chandra Sukma</t>
+  </si>
+  <si>
+    <t>2581065@student.vu.nl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +183,15 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -199,17 +217,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,20 +530,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -544,7 +565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -555,7 +576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -566,7 +587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -577,7 +598,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -588,7 +609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -599,7 +620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -610,7 +631,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -621,7 +642,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -632,7 +653,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -643,7 +664,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -654,7 +675,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -665,7 +686,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -676,8 +697,22 @@
         <v>41</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C15" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -693,7 +728,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -710,7 +745,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>